<commit_message>
update the Scan counting atoms and sorting the counts
</commit_message>
<xml_diff>
--- a/docs/atomUsage.xlsx
+++ b/docs/atomUsage.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="atomUsage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="123">
   <si>
     <t>hydrogen</t>
   </si>
@@ -377,6 +377,12 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Element 2nd pass</t>
+  </si>
+  <si>
+    <t>981 PDB files</t>
   </si>
 </sst>
 </file>
@@ -861,7 +867,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -871,6 +877,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1214,21 +1223,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>117</v>
       </c>
@@ -1238,8 +1250,17 @@
       <c r="C1" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1247,18 +1268,27 @@
         <v>5159699</v>
       </c>
       <c r="C2" s="3">
-        <f>B2/$E$2</f>
+        <f t="shared" ref="C2:C33" si="0">B2/$D$3</f>
         <v>0.59103365674840591</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="2">
-        <f>SUM(B:B)</f>
-        <v>8729958</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>5031539</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G33" si="1">F2/$D$3</f>
+        <v>0.57635317374951867</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1266,11 +1296,29 @@
         <v>1856606</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C66" si="0">B3/$E$2</f>
+        <f t="shared" si="0"/>
         <v>0.21267066806048782</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <f>SUM($B:$B)</f>
+        <v>8729958</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>1803267</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.20656078757767218</v>
+      </c>
+      <c r="H3" s="2">
+        <f>SUM($F:$F)</f>
+        <v>8501285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1281,8 +1329,21 @@
         <f t="shared" si="0"/>
         <v>0.16652233607538547</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>1411944</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.16173548601264748</v>
+      </c>
+      <c r="H4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1293,8 +1354,18 @@
         <f t="shared" si="0"/>
         <v>2.1682349445438339E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>189286</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1682349445438339E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1305,8 +1376,18 @@
         <f t="shared" si="0"/>
         <v>4.0595842500044102E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>34809</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9873044062754938E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1317,8 +1398,18 @@
         <f t="shared" si="0"/>
         <v>3.2657659979578365E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>25078</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="1"/>
+        <v>2.8726369588490575E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1329,8 +1420,18 @@
         <f t="shared" si="0"/>
         <v>3.9622183749337623E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>2598</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="1"/>
+        <v>2.975959334512262E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1341,8 +1442,18 @@
         <f t="shared" si="0"/>
         <v>7.1134362845731909E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>621</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="1"/>
+        <v>7.1134362845731909E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>75</v>
       </c>
@@ -1353,8 +1464,18 @@
         <f t="shared" si="0"/>
         <v>5.269212062646808E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>368</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="1"/>
+        <v>4.2153696501174458E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1365,8 +1486,18 @@
         <f t="shared" si="0"/>
         <v>4.2153696501174458E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11">
+        <v>328</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7571772968438107E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1377,8 +1508,18 @@
         <f t="shared" si="0"/>
         <v>3.7571772968438107E-5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>307</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="1"/>
+        <v>3.5166263113751518E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1389,8 +1530,18 @@
         <f t="shared" si="0"/>
         <v>3.5166263113751518E-5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>202</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="1"/>
+        <v>2.313871384031859E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1401,8 +1552,18 @@
         <f t="shared" si="0"/>
         <v>2.313871384031859E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>194</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2222329133771319E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1413,8 +1574,18 @@
         <f t="shared" si="0"/>
         <v>2.2222329133771319E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>187</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1420492515542457E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1425,8 +1596,18 @@
         <f t="shared" si="0"/>
         <v>2.1420492515542457E-5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>121</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3860318686527472E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1437,8 +1618,18 @@
         <f t="shared" si="0"/>
         <v>1.3974866774845882E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17">
+        <v>71</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="1"/>
+        <v>8.1329142706070295E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1449,8 +1640,18 @@
         <f t="shared" si="0"/>
         <v>8.1329142706070295E-6</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18">
+        <v>47</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="1"/>
+        <v>5.3837601509652166E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
@@ -1461,8 +1662,18 @@
         <f t="shared" si="0"/>
         <v>5.3837601509652166E-6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19">
+        <v>45</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="1"/>
+        <v>5.1546639743283988E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
@@ -1473,8 +1684,18 @@
         <f t="shared" si="0"/>
         <v>5.1546639743283988E-6</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="1"/>
+        <v>3.4364426495522658E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1485,8 +1706,18 @@
         <f t="shared" si="0"/>
         <v>3.4364426495522658E-6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>28</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="1"/>
+        <v>3.207346472915448E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1497,8 +1728,18 @@
         <f t="shared" si="0"/>
         <v>3.207346472915448E-6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22">
+        <v>28</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="1"/>
+        <v>3.207346472915448E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1509,8 +1750,18 @@
         <f t="shared" si="0"/>
         <v>3.207346472915448E-6</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23">
+        <v>27</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="1"/>
+        <v>3.0927983845970391E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1521,8 +1772,18 @@
         <f t="shared" si="0"/>
         <v>3.0927983845970391E-6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24">
+        <v>26</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="1"/>
+        <v>2.9782502962786303E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1533,8 +1794,18 @@
         <f t="shared" si="0"/>
         <v>2.9782502962786303E-6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="1"/>
+        <v>2.7491541196418125E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
@@ -1545,8 +1816,18 @@
         <f t="shared" si="0"/>
         <v>2.7491541196418125E-6</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26">
+        <v>16</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8327694130945417E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1557,8 +1838,18 @@
         <f t="shared" si="0"/>
         <v>1.8327694130945417E-6</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27">
+        <v>16</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8327694130945417E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
@@ -1569,8 +1860,18 @@
         <f t="shared" si="0"/>
         <v>1.8327694130945417E-6</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28">
+        <v>13</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4891251481393151E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1581,8 +1882,18 @@
         <f t="shared" si="0"/>
         <v>1.4891251481393151E-6</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29">
+        <v>13</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4891251481393151E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
@@ -1593,8 +1904,18 @@
         <f t="shared" si="0"/>
         <v>1.4891251481393151E-6</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30">
+        <v>11</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2600289715024974E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
@@ -1605,8 +1926,18 @@
         <f t="shared" si="0"/>
         <v>1.2600289715024974E-6</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0309327948656799E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -1617,8 +1948,18 @@
         <f t="shared" si="0"/>
         <v>1.0309327948656799E-6</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0309327948656799E-6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -1629,8 +1970,18 @@
         <f t="shared" si="0"/>
         <v>1.0309327948656799E-6</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="1"/>
+        <v>6.8728852991045313E-7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1638,11 +1989,21 @@
         <v>6</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C34:C65" si="2">B34/$D$3</f>
         <v>6.8728852991045313E-7</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" ref="G34:G65" si="3">F34/$D$3</f>
+        <v>3.4364426495522656E-7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
@@ -1650,11 +2011,21 @@
         <v>3</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.4364426495522656E-7</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4364426495522656E-7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
@@ -1662,11 +2033,21 @@
         <v>3</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.4364426495522656E-7</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" si="3"/>
+        <v>3.4364426495522656E-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
@@ -1674,11 +2055,21 @@
         <v>3</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.4364426495522656E-7</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" si="3"/>
+        <v>2.2909617663681772E-7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -1686,11 +2077,21 @@
         <v>2</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2909617663681772E-7</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" si="3"/>
+        <v>2.2909617663681772E-7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>22</v>
       </c>
@@ -1698,11 +2099,21 @@
         <v>2</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2909617663681772E-7</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="3"/>
+        <v>2.2909617663681772E-7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
@@ -1710,11 +2121,21 @@
         <v>2</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2909617663681772E-7</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1454808831840886E-7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -1722,11 +2143,21 @@
         <v>1</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1454808831840886E-7</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1454808831840886E-7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>91</v>
       </c>
@@ -1734,11 +2165,21 @@
         <v>1</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1454808831840886E-7</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
@@ -1746,11 +2187,21 @@
         <v>0</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -1758,11 +2209,21 @@
         <v>0</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
@@ -1770,11 +2231,21 @@
         <v>0</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -1782,11 +2253,21 @@
         <v>0</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>20</v>
       </c>
@@ -1794,11 +2275,21 @@
         <v>0</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -1806,11 +2297,21 @@
         <v>0</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -1818,11 +2319,21 @@
         <v>0</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>30</v>
       </c>
@@ -1830,11 +2341,21 @@
         <v>0</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>31</v>
       </c>
@@ -1842,11 +2363,21 @@
         <v>0</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>35</v>
       </c>
@@ -1854,11 +2385,21 @@
         <v>0</v>
       </c>
       <c r="C52" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>38</v>
       </c>
@@ -1866,11 +2407,21 @@
         <v>0</v>
       </c>
       <c r="C53" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>39</v>
       </c>
@@ -1878,11 +2429,21 @@
         <v>0</v>
       </c>
       <c r="C54" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>39</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>40</v>
       </c>
@@ -1890,11 +2451,21 @@
         <v>0</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>42</v>
       </c>
@@ -1902,11 +2473,21 @@
         <v>0</v>
       </c>
       <c r="C56" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>43</v>
       </c>
@@ -1914,11 +2495,21 @@
         <v>0</v>
       </c>
       <c r="C57" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>44</v>
       </c>
@@ -1926,11 +2517,21 @@
         <v>0</v>
       </c>
       <c r="C58" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>44</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>45</v>
       </c>
@@ -1938,11 +2539,21 @@
         <v>0</v>
       </c>
       <c r="C59" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>46</v>
       </c>
@@ -1950,11 +2561,21 @@
         <v>0</v>
       </c>
       <c r="C60" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
@@ -1962,11 +2583,21 @@
         <v>0</v>
       </c>
       <c r="C61" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>48</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>49</v>
       </c>
@@ -1974,11 +2605,21 @@
         <v>0</v>
       </c>
       <c r="C62" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>49</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>50</v>
       </c>
@@ -1986,11 +2627,21 @@
         <v>0</v>
       </c>
       <c r="C63" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>50</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>51</v>
       </c>
@@ -1998,11 +2649,21 @@
         <v>0</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>51</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>54</v>
       </c>
@@ -2010,11 +2671,21 @@
         <v>0</v>
       </c>
       <c r="C65" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>55</v>
       </c>
@@ -2022,11 +2693,21 @@
         <v>0</v>
       </c>
       <c r="C66" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" ref="C66:C97" si="4">B66/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>55</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3">
+        <f t="shared" ref="G66:G97" si="5">F66/$D$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>56</v>
       </c>
@@ -2034,11 +2715,21 @@
         <v>0</v>
       </c>
       <c r="C67" s="3">
-        <f t="shared" ref="C67:C118" si="1">B67/$E$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>56</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>57</v>
       </c>
@@ -2046,11 +2737,21 @@
         <v>0</v>
       </c>
       <c r="C68" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>57</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>58</v>
       </c>
@@ -2058,11 +2759,21 @@
         <v>0</v>
       </c>
       <c r="C69" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>58</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>59</v>
       </c>
@@ -2070,11 +2781,21 @@
         <v>0</v>
       </c>
       <c r="C70" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>59</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>60</v>
       </c>
@@ -2082,11 +2803,21 @@
         <v>0</v>
       </c>
       <c r="C71" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>60</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>62</v>
       </c>
@@ -2094,11 +2825,21 @@
         <v>0</v>
       </c>
       <c r="C72" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>62</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>63</v>
       </c>
@@ -2106,11 +2847,21 @@
         <v>0</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>63</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>64</v>
       </c>
@@ -2118,11 +2869,21 @@
         <v>0</v>
       </c>
       <c r="C74" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>64</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>65</v>
       </c>
@@ -2130,11 +2891,21 @@
         <v>0</v>
       </c>
       <c r="C75" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>65</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
@@ -2142,11 +2913,21 @@
         <v>0</v>
       </c>
       <c r="C76" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>66</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
@@ -2154,11 +2935,21 @@
         <v>0</v>
       </c>
       <c r="C77" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>67</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>68</v>
       </c>
@@ -2166,11 +2957,21 @@
         <v>0</v>
       </c>
       <c r="C78" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>68</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>70</v>
       </c>
@@ -2178,11 +2979,21 @@
         <v>0</v>
       </c>
       <c r="C79" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>70</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>71</v>
       </c>
@@ -2190,11 +3001,21 @@
         <v>0</v>
       </c>
       <c r="C80" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>71</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>72</v>
       </c>
@@ -2202,11 +3023,21 @@
         <v>0</v>
       </c>
       <c r="C81" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>72</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>73</v>
       </c>
@@ -2214,11 +3045,21 @@
         <v>0</v>
       </c>
       <c r="C82" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>73</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>74</v>
       </c>
@@ -2226,11 +3067,21 @@
         <v>0</v>
       </c>
       <c r="C83" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>74</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>77</v>
       </c>
@@ -2238,11 +3089,21 @@
         <v>0</v>
       </c>
       <c r="C84" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>75</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
@@ -2250,11 +3111,21 @@
         <v>0</v>
       </c>
       <c r="C85" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>77</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>82</v>
       </c>
@@ -2262,11 +3133,21 @@
         <v>0</v>
       </c>
       <c r="C86" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>80</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>83</v>
       </c>
@@ -2274,11 +3155,21 @@
         <v>0</v>
       </c>
       <c r="C87" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>82</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>84</v>
       </c>
@@ -2286,11 +3177,21 @@
         <v>0</v>
       </c>
       <c r="C88" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>83</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -2298,11 +3199,21 @@
         <v>0</v>
       </c>
       <c r="C89" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>84</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>86</v>
       </c>
@@ -2310,11 +3221,21 @@
         <v>0</v>
       </c>
       <c r="C90" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>85</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>87</v>
       </c>
@@ -2322,11 +3243,21 @@
         <v>0</v>
       </c>
       <c r="C91" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E91" t="s">
+        <v>86</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>88</v>
       </c>
@@ -2334,11 +3265,21 @@
         <v>0</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E92" t="s">
+        <v>87</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>89</v>
       </c>
@@ -2346,11 +3287,21 @@
         <v>0</v>
       </c>
       <c r="C93" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E93" t="s">
+        <v>88</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>90</v>
       </c>
@@ -2358,11 +3309,21 @@
         <v>0</v>
       </c>
       <c r="C94" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>89</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
@@ -2370,11 +3331,21 @@
         <v>0</v>
       </c>
       <c r="C95" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>90</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -2382,11 +3353,21 @@
         <v>0</v>
       </c>
       <c r="C96" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E96" t="s">
+        <v>92</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
@@ -2394,11 +3375,21 @@
         <v>0</v>
       </c>
       <c r="C97" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>94</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
@@ -2406,11 +3397,21 @@
         <v>0</v>
       </c>
       <c r="C98" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" ref="C98:C129" si="6">B98/$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>95</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98" s="3">
+        <f t="shared" ref="G98:G129" si="7">F98/$D$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -2418,11 +3419,21 @@
         <v>0</v>
       </c>
       <c r="C99" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>96</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -2430,11 +3441,21 @@
         <v>0</v>
       </c>
       <c r="C100" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E100" t="s">
+        <v>97</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
@@ -2442,11 +3463,21 @@
         <v>0</v>
       </c>
       <c r="C101" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E101" t="s">
+        <v>98</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -2454,11 +3485,21 @@
         <v>0</v>
       </c>
       <c r="C102" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E102" t="s">
+        <v>99</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
@@ -2466,11 +3507,21 @@
         <v>0</v>
       </c>
       <c r="C103" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E103" t="s">
+        <v>100</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -2478,11 +3529,21 @@
         <v>0</v>
       </c>
       <c r="C104" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E104" t="s">
+        <v>101</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
@@ -2490,11 +3551,21 @@
         <v>0</v>
       </c>
       <c r="C105" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>102</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -2502,11 +3573,21 @@
         <v>0</v>
       </c>
       <c r="C106" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E106" t="s">
+        <v>103</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
@@ -2514,11 +3595,21 @@
         <v>0</v>
       </c>
       <c r="C107" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E107" t="s">
+        <v>104</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -2526,11 +3617,21 @@
         <v>0</v>
       </c>
       <c r="C108" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E108" t="s">
+        <v>105</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
@@ -2538,11 +3639,21 @@
         <v>0</v>
       </c>
       <c r="C109" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E109" t="s">
+        <v>106</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -2550,11 +3661,21 @@
         <v>0</v>
       </c>
       <c r="C110" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E110" t="s">
+        <v>107</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
@@ -2562,11 +3683,21 @@
         <v>0</v>
       </c>
       <c r="C111" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>108</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
@@ -2574,11 +3705,21 @@
         <v>0</v>
       </c>
       <c r="C112" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E112" t="s">
+        <v>109</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
@@ -2586,11 +3727,21 @@
         <v>0</v>
       </c>
       <c r="C113" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E113" t="s">
+        <v>110</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -2598,11 +3749,21 @@
         <v>0</v>
       </c>
       <c r="C114" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E114" t="s">
+        <v>111</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -2610,11 +3771,21 @@
         <v>0</v>
       </c>
       <c r="C115" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E115" t="s">
+        <v>112</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
@@ -2622,11 +3793,21 @@
         <v>0</v>
       </c>
       <c r="C116" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E116" t="s">
+        <v>113</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
@@ -2634,11 +3815,21 @@
         <v>0</v>
       </c>
       <c r="C117" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E117" t="s">
+        <v>114</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
@@ -2646,7 +3837,17 @@
         <v>0</v>
       </c>
       <c r="C118" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E118" t="s">
+        <v>115</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118" s="3">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>